<commit_message>
Add llm prediction results
</commit_message>
<xml_diff>
--- a/Mitigation.xlsx
+++ b/Mitigation.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanwe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanwe\Desktop\Medline-grant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555DD161-E11D-4775-95D5-78064483668D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B2C13B-96A1-4492-ADEE-B0E13694A964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{911338DE-049E-8747-8024-3B6139CF33DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$233</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="997">
   <si>
     <t>File_path</t>
   </si>
@@ -3024,6 +3027,10 @@
   </si>
   <si>
     <t>tricky</t>
+  </si>
+  <si>
+    <t>ethanol + temazepam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3402,10 +3409,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434DDD9B-13E5-F147-A179-AEA155C0992B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N233"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="E248" sqref="E247:E248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3531,7 +3539,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>964</v>
       </c>
@@ -3569,7 +3577,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>964</v>
       </c>
@@ -3607,7 +3615,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>369</v>
       </c>
@@ -3645,7 +3653,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>369</v>
       </c>
@@ -3683,7 +3691,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>369</v>
       </c>
@@ -3721,7 +3729,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>369</v>
       </c>
@@ -3759,7 +3767,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>369</v>
       </c>
@@ -3855,7 +3863,7 @@
         <v>588</v>
       </c>
       <c r="G12" t="s">
-        <v>979</v>
+        <v>996</v>
       </c>
       <c r="H12" t="s">
         <v>23</v>
@@ -3873,7 +3881,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>937</v>
       </c>
@@ -3911,7 +3919,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>937</v>
       </c>
@@ -4025,7 +4033,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>190</v>
       </c>
@@ -4063,7 +4071,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>436</v>
       </c>
@@ -4101,7 +4109,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>436</v>
       </c>
@@ -4139,7 +4147,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>436</v>
       </c>
@@ -4177,7 +4185,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>436</v>
       </c>
@@ -4215,7 +4223,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>362</v>
       </c>
@@ -4253,7 +4261,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>907</v>
       </c>
@@ -4291,7 +4299,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>610</v>
       </c>
@@ -4329,7 +4337,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>224</v>
       </c>
@@ -4367,7 +4375,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>224</v>
       </c>
@@ -4405,7 +4413,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>224</v>
       </c>
@@ -4443,7 +4451,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>224</v>
       </c>
@@ -4481,7 +4489,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>224</v>
       </c>
@@ -4519,7 +4527,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>890</v>
       </c>
@@ -4557,7 +4565,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>314</v>
       </c>
@@ -4595,7 +4603,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -4633,7 +4641,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>694</v>
       </c>
@@ -4671,7 +4679,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>861</v>
       </c>
@@ -4709,7 +4717,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>861</v>
       </c>
@@ -4747,7 +4755,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -4785,7 +4793,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -4823,7 +4831,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -4861,7 +4869,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>102</v>
       </c>
@@ -4899,7 +4907,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -4937,7 +4945,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -4975,7 +4983,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>102</v>
       </c>
@@ -5013,7 +5021,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>200</v>
       </c>
@@ -5051,7 +5059,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>200</v>
       </c>
@@ -5089,7 +5097,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>532</v>
       </c>
@@ -5127,7 +5135,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -5165,7 +5173,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -5203,7 +5211,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>362</v>
       </c>
@@ -5241,7 +5249,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -5279,7 +5287,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>868</v>
       </c>
@@ -5317,7 +5325,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>278</v>
       </c>
@@ -5355,7 +5363,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>278</v>
       </c>
@@ -5393,7 +5401,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>278</v>
       </c>
@@ -5431,7 +5439,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>352</v>
       </c>
@@ -5469,7 +5477,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>352</v>
       </c>
@@ -5507,7 +5515,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>654</v>
       </c>
@@ -5545,7 +5553,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>265</v>
       </c>
@@ -5583,7 +5591,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>265</v>
       </c>
@@ -5621,7 +5629,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>265</v>
       </c>
@@ -5662,7 +5670,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>265</v>
       </c>
@@ -5703,7 +5711,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>45</v>
       </c>
@@ -5744,7 +5752,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -5785,7 +5793,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>937</v>
       </c>
@@ -5826,7 +5834,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>584</v>
       </c>
@@ -5864,7 +5872,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>159</v>
       </c>
@@ -5902,7 +5910,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>159</v>
       </c>
@@ -5940,7 +5948,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>126</v>
       </c>
@@ -5978,7 +5986,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>126</v>
       </c>
@@ -6016,7 +6024,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>436</v>
       </c>
@@ -6054,7 +6062,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>436</v>
       </c>
@@ -6092,7 +6100,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>436</v>
       </c>
@@ -6130,7 +6138,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>436</v>
       </c>
@@ -6168,7 +6176,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>436</v>
       </c>
@@ -6206,7 +6214,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>436</v>
       </c>
@@ -6244,7 +6252,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>291</v>
       </c>
@@ -6285,7 +6293,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>265</v>
       </c>
@@ -6326,7 +6334,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>484</v>
       </c>
@@ -6364,7 +6372,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>642</v>
       </c>
@@ -6402,7 +6410,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>907</v>
       </c>
@@ -6440,7 +6448,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -6478,7 +6486,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>314</v>
       </c>
@@ -6516,7 +6524,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>504</v>
       </c>
@@ -6554,7 +6562,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>230</v>
       </c>
@@ -6592,7 +6600,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>617</v>
       </c>
@@ -6633,7 +6641,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>387</v>
       </c>
@@ -6671,7 +6679,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>76</v>
       </c>
@@ -6709,7 +6717,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>806</v>
       </c>
@@ -6747,7 +6755,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>510</v>
       </c>
@@ -6785,7 +6793,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>510</v>
       </c>
@@ -6823,7 +6831,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>541</v>
       </c>
@@ -6861,7 +6869,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>436</v>
       </c>
@@ -6899,7 +6907,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>436</v>
       </c>
@@ -6937,7 +6945,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>38</v>
       </c>
@@ -6975,7 +6983,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>210</v>
       </c>
@@ -7013,7 +7021,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>324</v>
       </c>
@@ -7051,7 +7059,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>436</v>
       </c>
@@ -7089,7 +7097,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>664</v>
       </c>
@@ -7127,7 +7135,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -7165,7 +7173,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -7203,7 +7211,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>330</v>
       </c>
@@ -7241,7 +7249,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>330</v>
       </c>
@@ -7279,7 +7287,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>330</v>
       </c>
@@ -7317,7 +7325,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>974</v>
       </c>
@@ -7355,7 +7363,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>510</v>
       </c>
@@ -7393,7 +7401,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>551</v>
       </c>
@@ -7431,7 +7439,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>510</v>
       </c>
@@ -7472,7 +7480,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>387</v>
       </c>
@@ -7513,7 +7521,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>146</v>
       </c>
@@ -7554,7 +7562,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>532</v>
       </c>
@@ -7595,7 +7603,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -7636,7 +7644,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>617</v>
       </c>
@@ -7677,7 +7685,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>675</v>
       </c>
@@ -7718,7 +7726,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>352</v>
       </c>
@@ -7759,7 +7767,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>694</v>
       </c>
@@ -7797,7 +7805,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>210</v>
       </c>
@@ -7838,7 +7846,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>591</v>
       </c>
@@ -7876,7 +7884,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>591</v>
       </c>
@@ -7914,7 +7922,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>937</v>
       </c>
@@ -7952,7 +7960,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>400</v>
       </c>
@@ -7993,7 +8001,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>400</v>
       </c>
@@ -8031,7 +8039,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>400</v>
       </c>
@@ -8072,7 +8080,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>400</v>
       </c>
@@ -8110,7 +8118,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>210</v>
       </c>
@@ -8151,7 +8159,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>591</v>
       </c>
@@ -8189,7 +8197,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>694</v>
       </c>
@@ -8227,7 +8235,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>416</v>
       </c>
@@ -8265,7 +8273,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>591</v>
       </c>
@@ -8306,7 +8314,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>626</v>
       </c>
@@ -8344,7 +8352,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>626</v>
       </c>
@@ -8382,7 +8390,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>24</v>
       </c>
@@ -8423,7 +8431,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>416</v>
       </c>
@@ -8461,7 +8469,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>291</v>
       </c>
@@ -8499,7 +8507,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>291</v>
       </c>
@@ -8537,7 +8545,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>291</v>
       </c>
@@ -8575,7 +8583,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>494</v>
       </c>
@@ -8613,7 +8621,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>494</v>
       </c>
@@ -8651,7 +8659,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>494</v>
       </c>
@@ -8689,7 +8697,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>247</v>
       </c>
@@ -8727,7 +8735,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>626</v>
       </c>
@@ -8765,7 +8773,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>626</v>
       </c>
@@ -8806,7 +8814,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>591</v>
       </c>
@@ -8844,7 +8852,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>400</v>
       </c>
@@ -8885,7 +8893,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>102</v>
       </c>
@@ -8926,7 +8934,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>654</v>
       </c>
@@ -8964,7 +8972,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>146</v>
       </c>
@@ -9002,7 +9010,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>45</v>
       </c>
@@ -9040,7 +9048,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>577</v>
       </c>
@@ -9078,7 +9086,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>577</v>
       </c>
@@ -9116,7 +9124,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>190</v>
       </c>
@@ -9154,7 +9162,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>159</v>
       </c>
@@ -9195,7 +9203,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>159</v>
       </c>
@@ -9233,7 +9241,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>847</v>
       </c>
@@ -9271,7 +9279,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>847</v>
       </c>
@@ -9309,7 +9317,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>847</v>
       </c>
@@ -9347,7 +9355,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>847</v>
       </c>
@@ -9385,7 +9393,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>237</v>
       </c>
@@ -9423,7 +9431,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>694</v>
       </c>
@@ -9461,7 +9469,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>694</v>
       </c>
@@ -9499,7 +9507,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>806</v>
       </c>
@@ -9537,7 +9545,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>45</v>
       </c>
@@ -9578,7 +9586,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>265</v>
       </c>
@@ -9616,7 +9624,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>217</v>
       </c>
@@ -9654,7 +9662,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>217</v>
       </c>
@@ -9692,7 +9700,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>224</v>
       </c>
@@ -9730,7 +9738,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>224</v>
       </c>
@@ -9768,7 +9776,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>52</v>
       </c>
@@ -9806,7 +9814,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>52</v>
       </c>
@@ -9844,7 +9852,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>291</v>
       </c>
@@ -9882,7 +9890,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>291</v>
       </c>
@@ -9920,7 +9928,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>541</v>
       </c>
@@ -9958,7 +9966,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>563</v>
       </c>
@@ -9996,7 +10004,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>136</v>
       </c>
@@ -10034,7 +10042,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>62</v>
       </c>
@@ -10072,7 +10080,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>62</v>
       </c>
@@ -10110,7 +10118,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>664</v>
       </c>
@@ -10148,7 +10156,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>265</v>
       </c>
@@ -10186,7 +10194,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>217</v>
       </c>
@@ -10224,7 +10232,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>510</v>
       </c>
@@ -10262,7 +10270,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>510</v>
       </c>
@@ -10300,7 +10308,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>217</v>
       </c>
@@ -10338,7 +10346,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>217</v>
       </c>
@@ -10376,7 +10384,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>95</v>
       </c>
@@ -10414,7 +10422,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>210</v>
       </c>
@@ -10452,7 +10460,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>937</v>
       </c>
@@ -10490,7 +10498,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>416</v>
       </c>
@@ -10528,7 +10536,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>416</v>
       </c>
@@ -10566,7 +10574,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>974</v>
       </c>
@@ -10604,7 +10612,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>617</v>
       </c>
@@ -10642,7 +10650,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>675</v>
       </c>
@@ -10680,7 +10688,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>551</v>
       </c>
@@ -10718,7 +10726,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>685</v>
       </c>
@@ -10756,7 +10764,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>685</v>
       </c>
@@ -10794,7 +10802,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>278</v>
       </c>
@@ -10832,7 +10840,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>642</v>
       </c>
@@ -10870,7 +10878,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>146</v>
       </c>
@@ -10908,7 +10916,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>907</v>
       </c>
@@ -10946,7 +10954,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>436</v>
       </c>
@@ -10984,7 +10992,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>436</v>
       </c>
@@ -11022,7 +11030,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>436</v>
       </c>
@@ -11060,7 +11068,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>436</v>
       </c>
@@ -11098,7 +11106,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>436</v>
       </c>
@@ -11136,7 +11144,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>436</v>
       </c>
@@ -11174,7 +11182,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>436</v>
       </c>
@@ -11212,7 +11220,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>436</v>
       </c>
@@ -11250,7 +11258,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>570</v>
       </c>
@@ -11288,7 +11296,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>648</v>
       </c>
@@ -11326,7 +11334,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>217</v>
       </c>
@@ -11364,7 +11372,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>875</v>
       </c>
@@ -11402,7 +11410,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>504</v>
       </c>
@@ -11440,7 +11448,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>832</v>
       </c>
@@ -11478,7 +11486,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>541</v>
       </c>
@@ -11516,7 +11524,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>159</v>
       </c>
@@ -11554,7 +11562,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>159</v>
       </c>
@@ -11592,7 +11600,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>730</v>
       </c>
@@ -11630,7 +11638,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>484</v>
       </c>
@@ -11668,7 +11676,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>88</v>
       </c>
@@ -11706,7 +11714,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>278</v>
       </c>
@@ -11744,7 +11752,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>330</v>
       </c>
@@ -11782,7 +11790,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>330</v>
       </c>
@@ -11820,7 +11828,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>330</v>
       </c>
@@ -11858,7 +11866,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>136</v>
       </c>
@@ -11896,7 +11904,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>900</v>
       </c>
@@ -11934,7 +11942,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>247</v>
       </c>
@@ -11972,7 +11980,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>237</v>
       </c>
@@ -12010,7 +12018,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>494</v>
       </c>
@@ -12048,7 +12056,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>31</v>
       </c>
@@ -12086,7 +12094,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>31</v>
       </c>
@@ -12124,7 +12132,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>177</v>
       </c>
@@ -12162,7 +12170,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>177</v>
       </c>
@@ -12200,7 +12208,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>177</v>
       </c>
@@ -12238,7 +12246,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>387</v>
       </c>
@@ -12276,7 +12284,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>504</v>
       </c>
@@ -12314,7 +12322,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>217</v>
       </c>
@@ -12353,6 +12361,17 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N233" xr:uid="{434DDD9B-13E5-F147-A179-AEA155C0992B}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="(1968, 1970), the higher serum concentrations of penicillins and cephaloridine reached after administration of probenecid are due not only to slower renal elimination but also to an altered distribution in the body."/>
+        <filter val="Acetaminophen diminished the binding of theophylline to human serum by a net change of 5.7% (percentage increase in free drug fraction [FDF], 11.0%) at 662 micromol/L and by a net change of 7.1% (percentage increase in FDF, 13.7%) at 1324 micromol/L."/>
+        <filter val="Acid-catalyzed ethanolysis of temazepam in anhydrous and aqueous ethanol solutions."/>
+        <filter val="ADL 8-2698, a trans-3,4-dimethyl-4-(3-hydroxyphenyl) piperidine, prevents gastrointestinal effects of intravenous morphine without affecting analgesia."/>
+        <filter val="ADL-8-2698 is a novel peripherally restricted opioid antagonist that may selectively prevent opioid-induced gastrointestinal effects without reversing analgesia."/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L233">
     <sortCondition ref="C2:C233"/>
   </sortState>

</xml_diff>